<commit_message>
keep burning from bring average 2 points up
</commit_message>
<xml_diff>
--- a/analitics/adjust_strategy_test.xlsx
+++ b/analitics/adjust_strategy_test.xlsx
@@ -4,14 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51100" windowHeight="22240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51100" windowHeight="22240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="best strategies" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -8155,11 +8153,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2146073528"/>
-        <c:axId val="2146076648"/>
+        <c:axId val="2066775512"/>
+        <c:axId val="2066772568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2146073528"/>
+        <c:axId val="2066775512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8169,7 +8167,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146076648"/>
+        <c:crossAx val="2066772568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8177,7 +8175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2146076648"/>
+        <c:axId val="2066772568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="310.0"/>
@@ -8190,7 +8188,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146073528"/>
+        <c:crossAx val="2066775512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10.0"/>
@@ -8243,19 +8241,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="data"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8582,7 +8567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I376"/>
     </sheetView>
   </sheetViews>
@@ -23243,4 +23228,1942 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:13">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>137.375</v>
+      </c>
+      <c r="F2">
+        <v>294.375</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>119</v>
+      </c>
+      <c r="M2">
+        <v>243.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>142.75</v>
+      </c>
+      <c r="F3">
+        <v>299.375</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>131.875</v>
+      </c>
+      <c r="M3">
+        <v>278.375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>123.25</v>
+      </c>
+      <c r="F4">
+        <v>267.875</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>135.5</v>
+      </c>
+      <c r="M4">
+        <v>287.875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>133.5</v>
+      </c>
+      <c r="F5">
+        <v>284.875</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>128.75</v>
+      </c>
+      <c r="M5">
+        <v>276.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>143.375</v>
+      </c>
+      <c r="F6">
+        <v>283.5</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>152.875</v>
+      </c>
+      <c r="M6">
+        <v>297.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>139</v>
+      </c>
+      <c r="F7">
+        <v>280.125</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>133.375</v>
+      </c>
+      <c r="M7">
+        <v>286.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>136.75</v>
+      </c>
+      <c r="F8">
+        <v>293.625</v>
+      </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>144.75</v>
+      </c>
+      <c r="M8">
+        <v>292.375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>129</v>
+      </c>
+      <c r="F9">
+        <v>271.25</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>137.125</v>
+      </c>
+      <c r="M9">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>138.25</v>
+      </c>
+      <c r="F10">
+        <v>286</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>143.25</v>
+      </c>
+      <c r="M10">
+        <v>300.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>142.125</v>
+      </c>
+      <c r="F11">
+        <v>294.25</v>
+      </c>
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>141.125</v>
+      </c>
+      <c r="M11">
+        <v>286.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>138.875</v>
+      </c>
+      <c r="F12">
+        <v>293.5</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12">
+        <v>132.625</v>
+      </c>
+      <c r="M12">
+        <v>284.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>135.375</v>
+      </c>
+      <c r="F13">
+        <v>294.875</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <v>146.5</v>
+      </c>
+      <c r="M13">
+        <v>309.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>139.75</v>
+      </c>
+      <c r="F14">
+        <v>289.5</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <v>134.875</v>
+      </c>
+      <c r="M14">
+        <v>284.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>139</v>
+      </c>
+      <c r="F15">
+        <v>300.375</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>6</v>
+      </c>
+      <c r="L15">
+        <v>141.375</v>
+      </c>
+      <c r="M15">
+        <v>295.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>136.875</v>
+      </c>
+      <c r="F16">
+        <v>297.75</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <v>145.5</v>
+      </c>
+      <c r="M16">
+        <v>307.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>125.375</v>
+      </c>
+      <c r="F17">
+        <v>276.625</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <v>147.625</v>
+      </c>
+      <c r="M17">
+        <v>301.125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>134.875</v>
+      </c>
+      <c r="F18">
+        <v>290</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>7</v>
+      </c>
+      <c r="L18">
+        <v>133.375</v>
+      </c>
+      <c r="M18">
+        <v>285.625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>130.125</v>
+      </c>
+      <c r="F19">
+        <v>278</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>7</v>
+      </c>
+      <c r="L19">
+        <v>132.25</v>
+      </c>
+      <c r="M19">
+        <v>280.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>135.875</v>
+      </c>
+      <c r="F20">
+        <v>297</v>
+      </c>
+      <c r="H20">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>135.5</v>
+      </c>
+      <c r="M20">
+        <v>291.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>141.75</v>
+      </c>
+      <c r="F21">
+        <v>300.875</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <v>147.125</v>
+      </c>
+      <c r="M21">
+        <v>298.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>132.5</v>
+      </c>
+      <c r="F22">
+        <v>275.25</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>141.375</v>
+      </c>
+      <c r="M22">
+        <v>292.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>134.5</v>
+      </c>
+      <c r="F23">
+        <v>289</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>7</v>
+      </c>
+      <c r="L23">
+        <v>138.25</v>
+      </c>
+      <c r="M23">
+        <v>286.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>132.375</v>
+      </c>
+      <c r="F24">
+        <v>277.5</v>
+      </c>
+      <c r="H24">
+        <v>6</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>148.75</v>
+      </c>
+      <c r="M24">
+        <v>293.875</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>143.25</v>
+      </c>
+      <c r="F25">
+        <v>299.875</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>6</v>
+      </c>
+      <c r="L25">
+        <v>132</v>
+      </c>
+      <c r="M25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>142.625</v>
+      </c>
+      <c r="F26">
+        <v>308.75</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+      <c r="K26">
+        <v>7</v>
+      </c>
+      <c r="L26">
+        <v>132.25</v>
+      </c>
+      <c r="M26">
+        <v>283.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>136.25</v>
+      </c>
+      <c r="F27">
+        <v>291.125</v>
+      </c>
+      <c r="H27">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <v>5</v>
+      </c>
+      <c r="L27">
+        <v>153.5</v>
+      </c>
+      <c r="M27">
+        <v>302.125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>135.75</v>
+      </c>
+      <c r="F28">
+        <v>283.375</v>
+      </c>
+      <c r="H28">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
+      </c>
+      <c r="K28">
+        <v>8</v>
+      </c>
+      <c r="L28">
+        <v>141.125</v>
+      </c>
+      <c r="M28">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>136.5</v>
+      </c>
+      <c r="F29">
+        <v>289.875</v>
+      </c>
+      <c r="H29">
+        <v>7</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>5</v>
+      </c>
+      <c r="L29">
+        <v>139</v>
+      </c>
+      <c r="M29">
+        <v>294.875</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>135.75</v>
+      </c>
+      <c r="F30">
+        <v>291.125</v>
+      </c>
+      <c r="H30">
+        <v>6</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <v>5</v>
+      </c>
+      <c r="L30">
+        <v>143.25</v>
+      </c>
+      <c r="M30">
+        <v>299.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>144</v>
+      </c>
+      <c r="F31">
+        <v>300.5</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>3</v>
+      </c>
+      <c r="K31">
+        <v>6</v>
+      </c>
+      <c r="L31">
+        <v>133.875</v>
+      </c>
+      <c r="M31">
+        <v>293.375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>123</v>
+      </c>
+      <c r="F32">
+        <v>265.875</v>
+      </c>
+      <c r="H32">
+        <v>6</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="K32">
+        <v>8</v>
+      </c>
+      <c r="L32">
+        <v>128.5</v>
+      </c>
+      <c r="M32">
+        <v>278.875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>142.75</v>
+      </c>
+      <c r="F33">
+        <v>299.875</v>
+      </c>
+      <c r="H33">
+        <v>7</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>3</v>
+      </c>
+      <c r="K33">
+        <v>7</v>
+      </c>
+      <c r="L33">
+        <v>137.125</v>
+      </c>
+      <c r="M33">
+        <v>285.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>137.25</v>
+      </c>
+      <c r="F34">
+        <v>289.375</v>
+      </c>
+      <c r="H34">
+        <v>6</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>3</v>
+      </c>
+      <c r="K34">
+        <v>7</v>
+      </c>
+      <c r="L34">
+        <v>136.25</v>
+      </c>
+      <c r="M34">
+        <v>289.125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>141.5</v>
+      </c>
+      <c r="F35">
+        <v>305.125</v>
+      </c>
+      <c r="H35">
+        <v>7</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35">
+        <v>3</v>
+      </c>
+      <c r="K35">
+        <v>6</v>
+      </c>
+      <c r="L35">
+        <v>129.125</v>
+      </c>
+      <c r="M35">
+        <v>282.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>134</v>
+      </c>
+      <c r="F36">
+        <v>297.5</v>
+      </c>
+      <c r="H36">
+        <v>5</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>5</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <v>137.75</v>
+      </c>
+      <c r="M36">
+        <v>285.75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>139.375</v>
+      </c>
+      <c r="F37">
+        <v>292.125</v>
+      </c>
+      <c r="H37">
+        <v>5</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="K37">
+        <v>5</v>
+      </c>
+      <c r="L37">
+        <v>141.125</v>
+      </c>
+      <c r="M37">
+        <v>290.125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>137.875</v>
+      </c>
+      <c r="F38">
+        <v>303.375</v>
+      </c>
+      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>4</v>
+      </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
+      <c r="L38">
+        <v>143.375</v>
+      </c>
+      <c r="M38">
+        <v>296.375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>141.625</v>
+      </c>
+      <c r="F39">
+        <v>304.875</v>
+      </c>
+      <c r="H39">
+        <v>5</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+      <c r="K39">
+        <v>8</v>
+      </c>
+      <c r="L39">
+        <v>140.375</v>
+      </c>
+      <c r="M39">
+        <v>306.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>147</v>
+      </c>
+      <c r="F40">
+        <v>297.75</v>
+      </c>
+      <c r="H40">
+        <v>7</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40">
+        <v>8</v>
+      </c>
+      <c r="L40">
+        <v>143.25</v>
+      </c>
+      <c r="M40">
+        <v>294.875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>140</v>
+      </c>
+      <c r="F41">
+        <v>307</v>
+      </c>
+      <c r="H41">
+        <v>7</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <v>7</v>
+      </c>
+      <c r="L41">
+        <v>140</v>
+      </c>
+      <c r="M41">
+        <v>285.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>138.625</v>
+      </c>
+      <c r="F42">
+        <v>297.625</v>
+      </c>
+      <c r="H42">
+        <v>7</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>4</v>
+      </c>
+      <c r="K42">
+        <v>7</v>
+      </c>
+      <c r="L42">
+        <v>147.75</v>
+      </c>
+      <c r="M42">
+        <v>301.625</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>138.5</v>
+      </c>
+      <c r="F43">
+        <v>294.5</v>
+      </c>
+      <c r="H43">
+        <v>5</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>3</v>
+      </c>
+      <c r="K43">
+        <v>4</v>
+      </c>
+      <c r="L43">
+        <v>141.375</v>
+      </c>
+      <c r="M43">
+        <v>298.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>139.125</v>
+      </c>
+      <c r="F44">
+        <v>294.875</v>
+      </c>
+      <c r="H44">
+        <v>7</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>2</v>
+      </c>
+      <c r="K44">
+        <v>5</v>
+      </c>
+      <c r="L44">
+        <v>139.25</v>
+      </c>
+      <c r="M44">
+        <v>297.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>136.625</v>
+      </c>
+      <c r="F45">
+        <v>280</v>
+      </c>
+      <c r="H45">
+        <v>7</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
+        <v>6</v>
+      </c>
+      <c r="K45">
+        <v>8</v>
+      </c>
+      <c r="L45">
+        <v>141</v>
+      </c>
+      <c r="M45">
+        <v>302.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>140.5</v>
+      </c>
+      <c r="F46">
+        <v>301.875</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <v>3</v>
+      </c>
+      <c r="K46">
+        <v>5</v>
+      </c>
+      <c r="L46">
+        <v>135.375</v>
+      </c>
+      <c r="M46">
+        <v>294.375</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>131.75</v>
+      </c>
+      <c r="F47">
+        <v>284.25</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>4</v>
+      </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
+      <c r="L47">
+        <v>149.875</v>
+      </c>
+      <c r="M47">
+        <v>289.375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>143.625</v>
+      </c>
+      <c r="F48">
+        <v>289.375</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>4</v>
+      </c>
+      <c r="L48">
+        <v>145.875</v>
+      </c>
+      <c r="M48">
+        <v>297.375</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>135.625</v>
+      </c>
+      <c r="F49">
+        <v>280</v>
+      </c>
+      <c r="H49">
+        <v>7</v>
+      </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>5</v>
+      </c>
+      <c r="L49">
+        <v>143.375</v>
+      </c>
+      <c r="M49">
+        <v>288.875</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>140.375</v>
+      </c>
+      <c r="F50">
+        <v>299</v>
+      </c>
+      <c r="H50">
+        <v>6</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>5</v>
+      </c>
+      <c r="K50">
+        <v>6</v>
+      </c>
+      <c r="L50">
+        <v>139.125</v>
+      </c>
+      <c r="M50">
+        <v>295.25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51">
+        <v>6</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51">
+        <v>141.25</v>
+      </c>
+      <c r="F51">
+        <v>300.375</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>3</v>
+      </c>
+      <c r="K51">
+        <v>5</v>
+      </c>
+      <c r="L51">
+        <v>151.375</v>
+      </c>
+      <c r="M51">
+        <v>308.25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="E54">
+        <f>AVERAGE(E2:E53)</f>
+        <v>137.3425</v>
+      </c>
+      <c r="F54">
+        <f>AVERAGE(F2:F53)</f>
+        <v>291.29750000000001</v>
+      </c>
+      <c r="L54">
+        <f>AVERAGE(L2:L53)</f>
+        <v>139.58000000000001</v>
+      </c>
+      <c r="M54">
+        <f>AVERAGE(M2:M53)</f>
+        <v>291.29750000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>